<commit_message>
Myapp User, Board SQL
</commit_message>
<xml_diff>
--- a/myapp/app-server/data.xlsx
+++ b/myapp/app-server/data.xlsx
@@ -6,15 +6,15 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="users" r:id="rId6" sheetId="106"/>
-    <sheet name="boards" r:id="rId7" sheetId="107"/>
-    <sheet name="projects" r:id="rId5" sheetId="108"/>
+    <sheet name="users" r:id="rId6" sheetId="100"/>
+    <sheet name="boards" r:id="rId7" sheetId="101"/>
+    <sheet name="projects" r:id="rId5" sheetId="102"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5770" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5169" uniqueCount="142">
   <si>
     <t>no</t>
   </si>
@@ -382,16 +382,10 @@
     <t>24</t>
   </si>
   <si>
-    <t>user25x</t>
-  </si>
-  <si>
-    <t>user25x@test.com</t>
-  </si>
-  <si>
-    <t>0000</t>
-  </si>
-  <si>
-    <t>010-1234-1122</t>
+    <t>user25</t>
+  </si>
+  <si>
+    <t>user25@test.com</t>
   </si>
   <si>
     <t>25</t>
@@ -403,46 +397,49 @@
     <t>user26@test.com</t>
   </si>
   <si>
-    <t>010-1111-1126</t>
+    <t>26</t>
+  </si>
+  <si>
+    <t>user27</t>
+  </si>
+  <si>
+    <t>user27@test.com</t>
   </si>
   <si>
     <t>8</t>
   </si>
   <si>
-    <t>ggx</t>
-  </si>
-  <si>
-    <t>gxgx</t>
-  </si>
-  <si>
-    <t>2024-07-29 17:54:14</t>
-  </si>
-  <si>
-    <t>p7</t>
-  </si>
-  <si>
-    <t>2024-07-01</t>
-  </si>
-  <si>
-    <t>2024-07-07</t>
-  </si>
-  <si>
-    <t>23,12,5</t>
-  </si>
-  <si>
-    <t>p8</t>
-  </si>
-  <si>
-    <t>프로젝트1</t>
-  </si>
-  <si>
-    <t>2024-08-01</t>
-  </si>
-  <si>
-    <t>2024-08-08</t>
-  </si>
-  <si>
-    <t>5,1,2,20</t>
+    <t>hh</t>
+  </si>
+  <si>
+    <t>hhh</t>
+  </si>
+  <si>
+    <t>2024-07-29 17:31:12</t>
+  </si>
+  <si>
+    <t>ddxx</t>
+  </si>
+  <si>
+    <t>dddxxx</t>
+  </si>
+  <si>
+    <t>iii</t>
+  </si>
+  <si>
+    <t>iiii</t>
+  </si>
+  <si>
+    <t>2024-07-29 17:33:02</t>
+  </si>
+  <si>
+    <t>okok222</t>
+  </si>
+  <si>
+    <t>okokokokok</t>
+  </si>
+  <si>
+    <t>5,6,12,13</t>
   </si>
 </sst>
 </file>
@@ -485,9 +482,9 @@
 </styleSheet>
 </file>
 
-<file path=xl/worksheets/sheet106.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet100.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -716,104 +713,19 @@
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>105</v>
+        <v>127</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>112</v>
+        <v>128</v>
       </c>
       <c r="C14" t="s" s="0">
-        <v>113</v>
+        <v>129</v>
       </c>
       <c r="D14" t="s" s="0">
         <v>8</v>
       </c>
       <c r="E14" t="s" s="0">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s" s="0">
-        <v>108</v>
-      </c>
-      <c r="B15" t="s" s="0">
-        <v>109</v>
-      </c>
-      <c r="C15" t="s" s="0">
-        <v>110</v>
-      </c>
-      <c r="D15" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="E15" t="s" s="0">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s" s="0">
-        <v>114</v>
-      </c>
-      <c r="B16" t="s" s="0">
-        <v>115</v>
-      </c>
-      <c r="C16" t="s" s="0">
-        <v>116</v>
-      </c>
-      <c r="D16" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="E16" t="s" s="0">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s" s="0">
-        <v>117</v>
-      </c>
-      <c r="B17" t="s" s="0">
-        <v>118</v>
-      </c>
-      <c r="C17" t="s" s="0">
-        <v>119</v>
-      </c>
-      <c r="D17" t="s" s="0">
-        <v>120</v>
-      </c>
-      <c r="E17" t="s" s="0">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s" s="0">
-        <v>121</v>
-      </c>
-      <c r="B18" t="s" s="0">
-        <v>122</v>
-      </c>
-      <c r="C18" t="s" s="0">
-        <v>123</v>
-      </c>
-      <c r="D18" t="s" s="0">
-        <v>124</v>
-      </c>
-      <c r="E18" t="s" s="0">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="s" s="0">
-        <v>126</v>
-      </c>
-      <c r="B19" t="s" s="0">
-        <v>127</v>
-      </c>
-      <c r="C19" t="s" s="0">
-        <v>128</v>
-      </c>
-      <c r="D19" t="s" s="0">
-        <v>124</v>
-      </c>
-      <c r="E19" t="s" s="0">
-        <v>129</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -821,7 +733,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet107.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet101.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E8"/>
   <sheetViews>
@@ -865,33 +777,33 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>10</v>
+        <v>67</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>60</v>
+        <v>134</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>61</v>
+        <v>135</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>10</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>63</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="E4" t="s" s="0">
         <v>59</v>
@@ -899,33 +811,33 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>67</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="E5" t="s" s="0">
-        <v>59</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>14</v>
+        <v>101</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>71</v>
+        <v>102</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>72</v>
+        <v>103</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>73</v>
+        <v>104</v>
       </c>
       <c r="E6" t="s" s="0">
         <v>59</v>
@@ -933,36 +845,36 @@
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>18</v>
+        <v>130</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>74</v>
+        <v>131</v>
       </c>
       <c r="C7" t="s" s="0">
-        <v>75</v>
+        <v>132</v>
       </c>
       <c r="D7" t="s" s="0">
-        <v>76</v>
+        <v>133</v>
       </c>
       <c r="E7" t="s" s="0">
-        <v>5</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>130</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="C8" t="s" s="0">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="D8" t="s" s="0">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="E8" t="s" s="0">
-        <v>5</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -970,9 +882,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet108.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet102.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1040,122 +952,62 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>63</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="F4" t="s" s="0">
-        <v>92</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>67</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="D5" t="s" s="0">
+        <v>83</v>
+      </c>
+      <c r="E5" t="s" s="0">
         <v>84</v>
       </c>
-      <c r="E5" t="s" s="0">
-        <v>88</v>
-      </c>
       <c r="F5" t="s" s="0">
-        <v>10</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>14</v>
+        <v>101</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>94</v>
+        <v>139</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>87</v>
+        <v>140</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="E6" t="s" s="0">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="F6" t="s" s="0">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s" s="0">
-        <v>18</v>
-      </c>
-      <c r="B7" t="s" s="0">
-        <v>96</v>
-      </c>
-      <c r="C7" t="s" s="0">
-        <v>97</v>
-      </c>
-      <c r="D7" t="s" s="0">
-        <v>83</v>
-      </c>
-      <c r="E7" t="s" s="0">
-        <v>84</v>
-      </c>
-      <c r="F7" t="s" s="0">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s" s="0">
-        <v>101</v>
-      </c>
-      <c r="B8" t="s" s="0">
-        <v>134</v>
-      </c>
-      <c r="C8" t="s" s="0">
-        <v>135</v>
-      </c>
-      <c r="D8" t="s" s="0">
-        <v>135</v>
-      </c>
-      <c r="E8" t="s" s="0">
-        <v>136</v>
-      </c>
-      <c r="F8" t="s" s="0">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s" s="0">
-        <v>130</v>
-      </c>
-      <c r="B9" t="s" s="0">
-        <v>138</v>
-      </c>
-      <c r="C9" t="s" s="0">
-        <v>139</v>
-      </c>
-      <c r="D9" t="s" s="0">
-        <v>140</v>
-      </c>
-      <c r="E9" t="s" s="0">
         <v>141</v>
-      </c>
-      <c r="F9" t="s" s="0">
-        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>